<commit_message>
Actualizacion desde proyecto local sin perder historial
</commit_message>
<xml_diff>
--- a/output/planilla_emplea_modelo.xlsx
+++ b/output/planilla_emplea_modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\bolsa_empleo_admin\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218DE376-104E-4CBA-B938-A823FB3E2E0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A9BBBC-E900-4338-BC54-25D65B43DB73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="81">
   <si>
     <t xml:space="preserve">DIRECCIÓN GENERAL DE EMPLEO - DIRECCIÓN DE INTERMEDIACIÓN LABORAL 
 DEPARTAMENTO DE ORIENTACIÓN LABORAL </t>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t>TIPO MOVILIDAD</t>
+  </si>
+  <si>
+    <t>CIUDAD POSTULANTE</t>
+  </si>
+  <si>
+    <t>DEPARTAMENTO POSTULANTE</t>
   </si>
 </sst>
 </file>
@@ -572,6 +578,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -593,6 +617,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -602,12 +629,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -615,18 +636,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -634,9 +643,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1377,128 +1383,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="108" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
     </row>
     <row r="2" spans="1:22" ht="57" customHeight="1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
     </row>
     <row r="4" spans="1:22" ht="21.75" customHeight="1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
     </row>
     <row r="5" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="36"/>
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -3048,99 +3054,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="108" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
     </row>
     <row r="2" spans="1:15" ht="57" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
     </row>
     <row r="3" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
     </row>
     <row r="5" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
     </row>
     <row r="6" spans="1:15" ht="58.5" customHeight="1">
       <c r="A6" s="16" t="s">
@@ -3521,7 +3527,7 @@
   <dimension ref="A1:U209"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3548,129 +3554,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="108" customHeight="1">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
+      <c r="A1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
     </row>
     <row r="2" spans="1:21" s="3" customFormat="1" ht="57" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="36"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="43"/>
     </row>
     <row r="3" spans="1:21" s="3" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="48"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="32"/>
     </row>
     <row r="5" spans="1:21" s="3" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41" t="s">
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="44"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="32"/>
     </row>
     <row r="6" spans="1:21" s="3" customFormat="1" ht="58.5" customHeight="1">
       <c r="A6" s="16" t="s">
@@ -3685,55 +3691,55 @@
       <c r="D6" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="37" t="s">
+      <c r="F6" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="L6" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="O6" s="38" t="s">
+      <c r="O6" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="P6" s="38" t="s">
+      <c r="P6" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="Q6" s="38" t="s">
+      <c r="Q6" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="R6" s="38" t="s">
+      <c r="R6" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="S6" s="37" t="s">
+      <c r="S6" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="T6" s="37" t="s">
+      <c r="T6" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="U6" s="37" t="s">
+      <c r="U6" s="27" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3944,13 +3950,13 @@
     <row r="209" ht="50.1" customHeight="1"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A2:U2"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A3:U3"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="14" orientation="portrait" r:id="rId1"/>

</xml_diff>